<commit_message>
Nieuws op portaal en index pagina + tabs op portaal
</commit_message>
<xml_diff>
--- a/Uren Grenspoal - Stephan.xlsx
+++ b/Uren Grenspoal - Stephan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Datum</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Portaal (mailing) + contact + temp page</t>
+  </si>
+  <si>
+    <t>Portaal tabs + nieuws op index en portaal</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B2:B30)</f>
-        <v>13.5</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -519,9 +522,15 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="1">
+        <v>42382</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>

</xml_diff>

<commit_message>
Nieuws items stylen + DB connection
</commit_message>
<xml_diff>
--- a/Uren Grenspoal - Stephan.xlsx
+++ b/Uren Grenspoal - Stephan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Datum</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Portaal tabs + nieuws op index en portaal</t>
+  </si>
+  <si>
+    <t>Nieuws items stylen + mysql DB onlin zetten</t>
   </si>
 </sst>
 </file>
@@ -401,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +442,7 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B2:B30)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -535,9 +538,15 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="1">
+        <v>42394</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>

</xml_diff>

<commit_message>
DB changes + nieuws
</commit_message>
<xml_diff>
--- a/Uren Grenspoal - Stephan.xlsx
+++ b/Uren Grenspoal - Stephan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applications\XAMPP\htdocs\Grenspoal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Grenspoal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Datum</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Nieuws items stylen + mysql DB onlin zetten</t>
+  </si>
+  <si>
+    <t>Nieuws items editen (start)</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -140,9 +143,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -180,7 +183,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -252,7 +255,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -405,7 +408,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +445,7 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B2:B30)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -484,8 +487,8 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <f>SUM(B4:B10)</f>
-        <v>12</v>
+        <f>SUM(B4:B29)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -554,9 +557,15 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="1">
+        <v>42402</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>

</xml_diff>

<commit_message>
Styled controls + uren
</commit_message>
<xml_diff>
--- a/Uren Grenspoal - Stephan.xlsx
+++ b/Uren Grenspoal - Stephan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Nieuws items editen (start)</t>
+  </si>
+  <si>
+    <t>Thema aangepast, bugfixes en nieuws carousel slider</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +448,7 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B2:B30)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -488,7 +491,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2">
         <f>SUM(B4:B29)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -570,9 +573,15 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="1">
+        <v>42429</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>

</xml_diff>

<commit_message>
Uren + DB script
</commit_message>
<xml_diff>
--- a/Uren Grenspoal - Stephan.xlsx
+++ b/Uren Grenspoal - Stephan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Merge naar nieuwe webhost</t>
+  </si>
+  <si>
+    <t>Laatste fixes voor nieuws/stijl/menu</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +457,7 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B2:B30)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -497,7 +500,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2">
         <f>SUM(B4:B29)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -618,8 +621,15 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="1">
+        <v>42436</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>

</xml_diff>